<commit_message>
make directories if they don't exist
</commit_message>
<xml_diff>
--- a/data/figs/people/people.xlsx
+++ b/data/figs/people/people.xlsx
@@ -205,7 +205,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF1EE84"/>
+        <fgColor rgb="FF82C6BD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -217,109 +217,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8FFFF2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF95A97A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF827CEA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCD7C7B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF83E293"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7BB5FB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC2C8A9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE2ACC9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEDFDD2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF395A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF8BEF1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCD7E5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBAA8FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFAAF3BD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7CAEB4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD67AFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF967BA0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA698D3"/>
+        <fgColor rgb="FFB5DEFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA0FEA4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA7ACA8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA8982"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC47CC0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7E977E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6CCE1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCA8C3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCB798"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6FBDA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2F97A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB3A3E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF80FAE6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0A779"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF96D77F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDF3B7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF797CED"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF18FFD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>

</xml_diff>

<commit_message>
harvest default project time 6.4 hrs, forecast default time 8 hrs
</commit_message>
<xml_diff>
--- a/data/figs/people/people.xlsx
+++ b/data/figs/people/people.xlsx
@@ -232,133 +232,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBE94A3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF81FC8C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF819E7A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF787D8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF6DBFB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB481DC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD5C2E7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9CCAD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8AB5FD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFC7B96"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBBD07A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF94E9B9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE6A183"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9FCBE0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7EF3F8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8AA6BF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF937F99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD1F9C9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5EE7D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD19AFE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA2B995"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7B80F4"/>
+        <fgColor rgb="FF99B27B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC3C2AE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF482A4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAEF80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D3F8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF91FE81"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7CF6C6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7ED194"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9FAD7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBE4B3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB3DA8B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB0B2DD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD787E2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA7EFC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF849DAC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7FDEC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9ED8FD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7F80EE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB57C83"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBB284"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA37BC8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEC1EB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>

</xml_diff>